<commit_message>
Added dynamic column arrangements
</commit_message>
<xml_diff>
--- a/app/Vocab list.xlsx
+++ b/app/Vocab list.xlsx
@@ -16,11 +16,11 @@
   <definedNames>
     <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">Adjectives!$A$1:$E$118</definedName>
     <definedName hidden="1" localSheetId="8" name="_xlnm._FilterDatabase">Sheet1!$B$1:$J$210</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_0B4F0204_0A23_4B5E_B8E1_9250788672F4_.wvu.FilterData">Words!$A$2:$J$775</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_6E0C52AB_7A95_458F_A862_C394B287895C_.wvu.FilterData">Words!$A$2:$J$775</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{0B4F0204-0A23-4B5E-B8E1-9250788672F4}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{6E0C52AB-7A95-458F-A862-C394B287895C}" name="Filter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -20532,7 +20532,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{0B4F0204-0A23-4B5E-B8E1-9250788672F4}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{6E0C52AB-7A95-458F-A862-C394B287895C}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$2:$J$775">
         <filterColumn colId="2">
           <filters>

</xml_diff>